<commit_message>
Final commit for assignment.
</commit_message>
<xml_diff>
--- a/tests/A02_pixell_test_plan_chequing_account.xlsx
+++ b/tests/A02_pixell_test_plan_chequing_account.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Intermediate Software Development0315\2. Assignments\assignments\assignment_02\instructions\given_files\assignment_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1875869731f30720/Documents/RRC/Intermediate software development/Module1 Assigntment/isd_project/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2873F10E-F8B1-4F89-8CDF-A98B96DD770E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{2873F10E-F8B1-4F89-8CDF-A98B96DD770E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DA4DBFE-5892-492E-B7D6-E3EBC5498ECB}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="3555" windowWidth="25185" windowHeight="11415" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -249,6 +249,56 @@
   </si>
   <si>
     <t>Attributes are set to input values (ensure to test for superclass and subclass attributes)</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>(12345,678,1000.00,2024-10-1,300,0.10)</t>
+  </si>
+  <si>
+    <t>(12345,678,1000.00,date(2024,10,1),300,0.10)</t>
+  </si>
+  <si>
+    <t>(12345,678,1000.00,date(2024,10,1),invalid type,0.10)</t>
+  </si>
+  <si>
+    <t>(12345,678,1000.00,date(2024,10,1),-100,0.10)</t>
+  </si>
+  <si>
+    <t>(12345,678,1000.00,date(2024,10,1),300,invalid rate)</t>
+  </si>
+  <si>
+    <t>(12345,678,1000.00,date(2024,10,1),300,0.05)</t>
+  </si>
+  <si>
+    <t>(12345,678,1000.00,invalid date,300,0.10)</t>
+  </si>
+  <si>
+    <t>(12345,678,1000.00,date.today(),300,0.10)</t>
+  </si>
+  <si>
+    <t>(12345,678,200.00,date(2024,10,1),300,0.10)</t>
+  </si>
+  <si>
+    <t>service charge = base service charge</t>
+  </si>
+  <si>
+    <t>service charge is correctly calculated base on the fomula</t>
+  </si>
+  <si>
+    <t>(12345,678,300.00,date(2024,10,1),300,0.10)</t>
+  </si>
+  <si>
+    <t>service charge equal to base service charge</t>
+  </si>
+  <si>
+    <t>str(self.chequeaccount1)</t>
+  </si>
+  <si>
+    <t>("Account Number: 12345 Balance: $1000.00"
+                        "\nOverdraft Limit: $300.00 Overdraft Rate: 10.00%"
+                        "\nAccount Type: Chequing")</t>
   </si>
 </sst>
 </file>
@@ -612,7 +662,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
@@ -836,7 +886,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1155,21 +1205,21 @@
   <dimension ref="B1:G32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B30"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="48.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="4" max="4" width="32.7265625" customWidth="1"/>
+    <col min="5" max="5" width="31.54296875" customWidth="1"/>
+    <col min="6" max="6" width="41.90625" customWidth="1"/>
+    <col min="7" max="7" width="48.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="2.15">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -1181,14 +1231,14 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1197,10 +1247,10 @@
       </c>
       <c r="D4" s="19"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="11">
         <v>1</v>
       </c>
@@ -1230,11 +1280,17 @@
       <c r="D7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="3">
         <v>2</v>
       </c>
@@ -1244,11 +1300,17 @@
       <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="11">
         <v>3</v>
       </c>
@@ -1258,11 +1320,17 @@
       <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="11">
         <v>4</v>
       </c>
@@ -1272,11 +1340,17 @@
       <c r="D10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="3">
         <v>5</v>
       </c>
@@ -1286,11 +1360,17 @@
       <c r="D11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="11">
         <v>6</v>
       </c>
@@ -1300,11 +1380,17 @@
       <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="11">
         <v>7</v>
       </c>
@@ -1314,11 +1400,17 @@
       <c r="D13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="2:7" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="3">
         <v>8</v>
       </c>
@@ -1328,11 +1420,17 @@
       <c r="D14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="11">
         <v>9</v>
       </c>
@@ -1342,7 +1440,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="11">
         <v>10</v>
       </c>
@@ -1352,7 +1450,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="3">
         <v>11</v>
       </c>
@@ -1362,7 +1460,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="11">
         <v>12</v>
       </c>
@@ -1372,7 +1470,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="11">
         <v>13</v>
       </c>
@@ -1382,7 +1480,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="3">
         <v>14</v>
       </c>
@@ -1392,7 +1490,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="11">
         <v>15</v>
       </c>
@@ -1402,7 +1500,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="11">
         <v>16</v>
       </c>
@@ -1412,7 +1510,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="3">
         <v>17</v>
       </c>
@@ -1422,7 +1520,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="11">
         <v>18</v>
       </c>
@@ -1432,7 +1530,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="11">
         <v>19</v>
       </c>
@@ -1442,7 +1540,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="3">
         <v>20</v>
       </c>
@@ -1452,7 +1550,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="11">
         <v>21</v>
       </c>
@@ -1462,7 +1560,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="11">
         <v>22</v>
       </c>
@@ -1472,7 +1570,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="3">
         <v>23</v>
       </c>
@@ -1482,7 +1580,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="11">
         <v>24</v>
       </c>
@@ -1492,7 +1590,7 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B32" s="20" t="s">
         <v>6</v>
       </c>

</xml_diff>